<commit_message>
Dodan okvir za tabele u excelu i napravljeni pdf
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/CaseOdobravanjeZahtjeva.xlsx
+++ b/UseCaseIScenarij/CaseOdobravanjeZahtjeva.xlsx
@@ -94,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,13 +102,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +432,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +441,7 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -437,76 +453,120 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preimenovano Baza podataka -> Analiza sadržaja
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/CaseOdobravanjeZahtjeva.xlsx
+++ b/UseCaseIScenarij/CaseOdobravanjeZahtjeva.xlsx
@@ -28,9 +28,6 @@
     <t>Administrator</t>
   </si>
   <si>
-    <t>Baza podataka</t>
-  </si>
-  <si>
     <t>1. Opis artikla koji se dodaje</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>3. Zahtjev (nije odobren)</t>
+  </si>
+  <si>
+    <t>Analiza sadržaja</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -469,15 +469,15 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -490,13 +490,13 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -505,7 +505,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -517,21 +517,21 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -540,7 +540,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -553,13 +553,13 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>

</xml_diff>